<commit_message>
improve layout of app
</commit_message>
<xml_diff>
--- a/examplefiles/annotations_combined/agreement_table.xlsx
+++ b/examplefiles/annotations_combined/agreement_table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14445" windowHeight="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14445" windowHeight="1538"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>VS06</t>
+  </si>
+  <si>
+    <t>VS08</t>
+  </si>
+  <si>
+    <t>VS24</t>
+  </si>
+  <si>
+    <t>sub-PD06</t>
+  </si>
+  <si>
+    <t>sub-PD10</t>
+  </si>
   <si>
     <t>filename</t>
   </si>
@@ -38,12 +56,6 @@
   </si>
   <si>
     <t>VS24_823</t>
-  </si>
-  <si>
-    <t>sub-PD06</t>
-  </si>
-  <si>
-    <t>sub-PD10</t>
   </si>
   <si>
     <t>TOTAL</t>
@@ -412,389 +424,408 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.06640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.53125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.53125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="17.06640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="25.73046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.19921875" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.06640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.53125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.53125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="17.06640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.59765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="25.73046875" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.19921875" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="J1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="K1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="L1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="M1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="N1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="O1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="P1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="Q1" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="R1" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
         <v>0.93846304086352705</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>0.698401158387709</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>0.66108018537645097</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>0.5</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0.33333333333333298</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>15</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>14</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>12</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>7</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>5</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>408.96699999999998</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>400.09699999999998</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>379.59</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>29.391999999999999</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>20.388999999999999</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>487.00900000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
         <v>0.82079680583282699</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>0.68870058200898598</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0.26930789061983601</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>0.84615384615384603</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>1</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>10</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>19</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>13</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>3</v>
       </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
       <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
         <v>98.236000000000004</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>74.55</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>70.923000000000002</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>27.323</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>3.6459999999999999</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>136.149</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
         <v>0.31275109170305698</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>0.88947412775998602</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>-0.72291459961764604</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>1</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0.5</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>6</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>3</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>2</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>4</v>
       </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
       <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
         <v>17.893000000000001</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>4.9989999999999997</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>3.581</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>14.317</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>1.421</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>82.646000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>0</v>
+      <c r="B5" t="s">
+        <v>4</v>
       </c>
       <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
         <v>0.99223127936492805</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>-0.98458233426777497</v>
       </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
       <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
         <v>9</v>
       </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
         <v>9</v>
       </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
       <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
         <v>25.081</v>
       </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
         <v>25.09</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>1627.354</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
         <v>0.56602029570582701</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>0.963435921756567</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>-0.84458798691910897</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>0.75</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>0.91666666666666696</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>15</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>17</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>12</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>4</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>14</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>84.583999999999804</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>168.541</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>71.646000000000001</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>12.952999999999999</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>96.912000000000006</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>1628.941</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
         <v>0.81959712313209776</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>0.96515081817873827</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>-0.67620117518517342</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>0.58417139504464033</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>0.50389736371590499</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>46</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>62</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>39</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>18</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>28</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>609.67999999999984</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>673.26800000000003</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>525.74</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>83.985000000000014</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>147.458</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>3962.0990000000002</v>
       </c>
     </row>

</xml_diff>

<commit_message>
save files which need revision in separate folder
</commit_message>
<xml_diff>
--- a/examplefiles/annotations_combined/agreement_table.xlsx
+++ b/examplefiles/annotations_combined/agreement_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\helen\Documents\1.Projects\FOG_annotation\FOGtool\examplefiles\annotations_combined\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9F565CA-5226-4B29-9E9A-9F0B28A0BFCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1DA149BA-930A-47E2-A10C-6F8DD206D58B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39870" yWindow="5510" windowWidth="19200" windowHeight="10050" xr2:uid="{1314A2A1-DAF2-4C84-9E54-5BA05075BAB0}"/>
+    <workbookView xWindow="39870" yWindow="5510" windowWidth="19200" windowHeight="10050" xr2:uid="{33C9F073-03D1-49AB-8072-4373F89912C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -468,7 +468,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D8253A5-332B-4B20-93BE-172DC2A4993B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92FB5BFA-7E4E-47CE-B2BD-6AD85F25A9F7}">
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -883,7 +883,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CB57A5F-0BB9-4885-8F2A-19F2B0B453BF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B530ACD8-856D-4141-B38E-E22F08F42631}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -895,7 +895,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1D9B482-0934-4FF1-B4D9-9451C2A04E4F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D037B1C-D3FB-4D15-9F40-B6774D620E79}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>